<commit_message>
New rule: All functional test data of all types must be found by q=__TEST__. This will make it easier to clean up later.
</commit_message>
<xml_diff>
--- a/YoFi.Tests.Functional/SampleData/Test-Generator-GenerateUploadSampleData.xlsx
+++ b/YoFi.Tests.Functional/SampleData/Test-Generator-GenerateUploadSampleData.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Transaction" sheetId="1" r:id="Rd62d74dc87614074"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Split" sheetId="2" r:id="R8f7a3d4d12a447f1"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Payee" sheetId="3" r:id="Rbbf8a40efbca4c61"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BudgetTx" sheetId="4" r:id="Rf917b239649640f0"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Transaction" sheetId="1" r:id="Rf8e98ca7f4db4c10"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Split" sheetId="2" r:id="R061bd591c405421a"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Payee" sheetId="3" r:id="Rc940b2989c3c45ce"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BudgetTx" sheetId="4" r:id="Ra9a48f6271854147"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -55,19 +55,19 @@
     <x:t>IsSplitsOK</x:t>
   </x:si>
   <x:si>
-    <x:t>Big Stuff</x:t>
-  </x:si>
-  <x:si>
-    <x:t>A:B</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Big Money</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Big Dogs</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:D</x:t>
+    <x:t>AA__TEST__2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AA:__TEST__:C</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AA__TEST__1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AA__TEST__3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AA:__TEST__:D</x:t>
   </x:si>
   <x:si>
     <x:t>SubCategory</x:t>
@@ -79,10 +79,10 @@
     <x:t>Transaction</x:t>
   </x:si>
   <x:si>
-    <x:t>X:Y</x:t>
-  </x:si>
-  <x:si>
-    <x:t>X:Z</x:t>
+    <x:t>AA:__TEST__:A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AA:__TEST__:B</x:t>
   </x:si>
   <x:si>
     <x:t>Name</x:t>
@@ -174,7 +174,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="B2" s="1" t="n">
-        <x:v>44210</x:v>
+        <x:v>44214</x:v>
       </x:c>
       <x:c r="C2" t="s">
         <x:v>14</x:v>
@@ -197,7 +197,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="B3" s="1" t="n">
-        <x:v>44212</x:v>
+        <x:v>44223</x:v>
       </x:c>
       <x:c r="C3" t="s">
         <x:v>16</x:v>
@@ -217,16 +217,16 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="B4" s="1" t="n">
-        <x:v>44241</x:v>
+        <x:v>44230</x:v>
       </x:c>
       <x:c r="C4" t="s">
-        <x:v>14</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="D4" s="2" t="n">
-        <x:v>-250</x:v>
+        <x:v>-4000</x:v>
       </x:c>
       <x:c r="E4" t="s">
-        <x:v>15</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="M4" t="b">
         <x:v>0</x:v>
@@ -237,19 +237,22 @@
     </x:row>
     <x:row r="5" spans="">
       <x:c r="A5" t="n">
-        <x:v>2</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="B5" s="1" t="n">
-        <x:v>44243</x:v>
+        <x:v>44245</x:v>
       </x:c>
       <x:c r="C5" t="s">
-        <x:v>16</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="D5" s="2" t="n">
-        <x:v>-250.00</x:v>
+        <x:v>-250</x:v>
+      </x:c>
+      <x:c r="E5" t="s">
+        <x:v>15</x:v>
       </x:c>
       <x:c r="M5" t="b">
-        <x:v>1</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="N5" t="b">
         <x:v>1</x:v>
@@ -257,22 +260,19 @@
     </x:row>
     <x:row r="6" spans="">
       <x:c r="A6" t="n">
-        <x:v>0</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="B6" s="1" t="n">
-        <x:v>44269</x:v>
+        <x:v>44254</x:v>
       </x:c>
       <x:c r="C6" t="s">
-        <x:v>14</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="D6" s="2" t="n">
-        <x:v>-250</x:v>
-      </x:c>
-      <x:c r="E6" t="s">
-        <x:v>15</x:v>
+        <x:v>-250.00</x:v>
       </x:c>
       <x:c r="M6" t="b">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="N6" t="b">
         <x:v>1</x:v>
@@ -280,19 +280,22 @@
     </x:row>
     <x:row r="7" spans="">
       <x:c r="A7" t="n">
-        <x:v>3</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="B7" s="1" t="n">
-        <x:v>44271</x:v>
+        <x:v>44273</x:v>
       </x:c>
       <x:c r="C7" t="s">
-        <x:v>16</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="D7" s="2" t="n">
-        <x:v>-250.00</x:v>
+        <x:v>-250</x:v>
+      </x:c>
+      <x:c r="E7" t="s">
+        <x:v>15</x:v>
       </x:c>
       <x:c r="M7" t="b">
-        <x:v>1</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="N7" t="b">
         <x:v>1</x:v>
@@ -300,22 +303,19 @@
     </x:row>
     <x:row r="8" spans="">
       <x:c r="A8" t="n">
-        <x:v>0</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B8" s="1" t="n">
-        <x:v>44300</x:v>
+        <x:v>44282</x:v>
       </x:c>
       <x:c r="C8" t="s">
-        <x:v>14</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="D8" s="2" t="n">
-        <x:v>-250</x:v>
-      </x:c>
-      <x:c r="E8" t="s">
-        <x:v>15</x:v>
+        <x:v>-250.00</x:v>
       </x:c>
       <x:c r="M8" t="b">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="N8" t="b">
         <x:v>1</x:v>
@@ -323,19 +323,22 @@
     </x:row>
     <x:row r="9" spans="">
       <x:c r="A9" t="n">
-        <x:v>4</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="B9" s="1" t="n">
-        <x:v>44302</x:v>
+        <x:v>44304</x:v>
       </x:c>
       <x:c r="C9" t="s">
-        <x:v>16</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="D9" s="2" t="n">
-        <x:v>-250.00</x:v>
+        <x:v>-250</x:v>
+      </x:c>
+      <x:c r="E9" t="s">
+        <x:v>15</x:v>
       </x:c>
       <x:c r="M9" t="b">
-        <x:v>1</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="N9" t="b">
         <x:v>1</x:v>
@@ -343,22 +346,19 @@
     </x:row>
     <x:row r="10" spans="">
       <x:c r="A10" t="n">
-        <x:v>0</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B10" s="1" t="n">
-        <x:v>44330</x:v>
+        <x:v>44313</x:v>
       </x:c>
       <x:c r="C10" t="s">
-        <x:v>14</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="D10" s="2" t="n">
-        <x:v>-250</x:v>
-      </x:c>
-      <x:c r="E10" t="s">
-        <x:v>15</x:v>
+        <x:v>-250.00</x:v>
       </x:c>
       <x:c r="M10" t="b">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="N10" t="b">
         <x:v>1</x:v>
@@ -366,19 +366,22 @@
     </x:row>
     <x:row r="11" spans="">
       <x:c r="A11" t="n">
-        <x:v>5</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="B11" s="1" t="n">
-        <x:v>44332</x:v>
+        <x:v>44334</x:v>
       </x:c>
       <x:c r="C11" t="s">
-        <x:v>16</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="D11" s="2" t="n">
-        <x:v>-250.00</x:v>
+        <x:v>-250</x:v>
+      </x:c>
+      <x:c r="E11" t="s">
+        <x:v>15</x:v>
       </x:c>
       <x:c r="M11" t="b">
-        <x:v>1</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="N11" t="b">
         <x:v>1</x:v>
@@ -386,22 +389,19 @@
     </x:row>
     <x:row r="12" spans="">
       <x:c r="A12" t="n">
-        <x:v>0</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B12" s="1" t="n">
-        <x:v>44361</x:v>
+        <x:v>44343</x:v>
       </x:c>
       <x:c r="C12" t="s">
-        <x:v>14</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="D12" s="2" t="n">
-        <x:v>-250</x:v>
-      </x:c>
-      <x:c r="E12" t="s">
-        <x:v>15</x:v>
+        <x:v>-250.00</x:v>
       </x:c>
       <x:c r="M12" t="b">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="N12" t="b">
         <x:v>1</x:v>
@@ -409,19 +409,22 @@
     </x:row>
     <x:row r="13" spans="">
       <x:c r="A13" t="n">
-        <x:v>6</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="B13" s="1" t="n">
-        <x:v>44363</x:v>
+        <x:v>44365</x:v>
       </x:c>
       <x:c r="C13" t="s">
-        <x:v>16</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="D13" s="2" t="n">
-        <x:v>-250.00</x:v>
+        <x:v>-250</x:v>
+      </x:c>
+      <x:c r="E13" t="s">
+        <x:v>15</x:v>
       </x:c>
       <x:c r="M13" t="b">
-        <x:v>1</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="N13" t="b">
         <x:v>1</x:v>
@@ -429,22 +432,19 @@
     </x:row>
     <x:row r="14" spans="">
       <x:c r="A14" t="n">
-        <x:v>0</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B14" s="1" t="n">
-        <x:v>44381</x:v>
+        <x:v>44374</x:v>
       </x:c>
       <x:c r="C14" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="D14" s="2" t="n">
-        <x:v>-4000</x:v>
-      </x:c>
-      <x:c r="E14" t="s">
-        <x:v>18</x:v>
+        <x:v>-250.00</x:v>
       </x:c>
       <x:c r="M14" t="b">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="N14" t="b">
         <x:v>1</x:v>
@@ -455,7 +455,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="B15" s="1" t="n">
-        <x:v>44391</x:v>
+        <x:v>44395</x:v>
       </x:c>
       <x:c r="C15" t="s">
         <x:v>14</x:v>
@@ -478,7 +478,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B16" s="1" t="n">
-        <x:v>44393</x:v>
+        <x:v>44404</x:v>
       </x:c>
       <x:c r="C16" t="s">
         <x:v>16</x:v>
@@ -498,7 +498,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="B17" s="1" t="n">
-        <x:v>44422</x:v>
+        <x:v>44426</x:v>
       </x:c>
       <x:c r="C17" t="s">
         <x:v>14</x:v>
@@ -521,7 +521,7 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="B18" s="1" t="n">
-        <x:v>44424</x:v>
+        <x:v>44435</x:v>
       </x:c>
       <x:c r="C18" t="s">
         <x:v>16</x:v>
@@ -541,7 +541,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="B19" s="1" t="n">
-        <x:v>44453</x:v>
+        <x:v>44457</x:v>
       </x:c>
       <x:c r="C19" t="s">
         <x:v>14</x:v>
@@ -564,7 +564,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="B20" s="1" t="n">
-        <x:v>44455</x:v>
+        <x:v>44466</x:v>
       </x:c>
       <x:c r="C20" t="s">
         <x:v>16</x:v>
@@ -584,7 +584,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="B21" s="1" t="n">
-        <x:v>44483</x:v>
+        <x:v>44487</x:v>
       </x:c>
       <x:c r="C21" t="s">
         <x:v>14</x:v>
@@ -607,7 +607,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="B22" s="1" t="n">
-        <x:v>44485</x:v>
+        <x:v>44496</x:v>
       </x:c>
       <x:c r="C22" t="s">
         <x:v>16</x:v>
@@ -627,7 +627,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="B23" s="1" t="n">
-        <x:v>44514</x:v>
+        <x:v>44518</x:v>
       </x:c>
       <x:c r="C23" t="s">
         <x:v>14</x:v>
@@ -650,7 +650,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="B24" s="1" t="n">
-        <x:v>44516</x:v>
+        <x:v>44527</x:v>
       </x:c>
       <x:c r="C24" t="s">
         <x:v>16</x:v>
@@ -670,7 +670,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="B25" s="1" t="n">
-        <x:v>44544</x:v>
+        <x:v>44548</x:v>
       </x:c>
       <x:c r="C25" t="s">
         <x:v>14</x:v>
@@ -693,7 +693,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="B26" s="1" t="n">
-        <x:v>44546</x:v>
+        <x:v>44557</x:v>
       </x:c>
       <x:c r="C26" t="s">
         <x:v>16</x:v>

</xml_diff>